<commit_message>
fix query allData: using RIGHT OUTER JOIN instead LEFT JOIN for count groups without students
</commit_message>
<xml_diff>
--- a/pivot.xlsx
+++ b/pivot.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>student_id</t>
   </si>
@@ -215,86 +215,96 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:L7" sheet="Лист1"/>
+    <worksheetSource ref="A1:L8" sheet="Лист1"/>
   </cacheSource>
   <cacheFields>
     <cacheField name="student_id" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1">
         <n v="1.0"/>
         <n v="2.0"/>
         <n v="3.0"/>
         <n v="4.0"/>
         <n v="5.0"/>
         <n v="6.0"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="firstName" numFmtId="0">
-      <sharedItems>
+      <sharedItems containsBlank="1">
         <s v="Иван"/>
         <s v="Наталья"/>
         <s v="Виктор"/>
         <s v="Петр"/>
         <s v="Вероника"/>
         <s v="Ирина"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="surName" numFmtId="0">
-      <sharedItems>
+      <sharedItems containsBlank="1">
         <s v="Степанов"/>
         <s v="Чичикова"/>
         <s v="Белов"/>
         <s v="Сушкин"/>
         <s v="Ковалева"/>
         <s v="Истомина"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="patronymic" numFmtId="0">
-      <sharedItems>
+      <sharedItems containsBlank="1">
         <s v="Сергеевич"/>
         <s v="Андреевна"/>
         <s v="Сидорович"/>
         <s v="Викторович"/>
         <s v="Сергеевна"/>
         <s v="Федоровна"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="dateOfBirth" numFmtId="0">
-      <sharedItems>
+      <sharedItems containsBlank="1">
         <s v="March, 20 1990 00:00:00"/>
         <s v="June, 10 1990 00:00:00"/>
         <s v="January, 10 1990 00:00:00"/>
         <s v="March, 12 1991 00:00:00"/>
         <s v="July, 19 1991 00:00:00"/>
         <s v="April, 29 1991 00:00:00"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="sex" numFmtId="0">
-      <sharedItems>
+      <sharedItems containsBlank="1">
         <s v="М"/>
         <s v="Ж"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="group_id" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1">
         <n v="1.0"/>
         <n v="2.0"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="educationYear" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1">
         <n v="2006.0"/>
+        <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="group_id2" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1">
         <n v="1.0"/>
         <n v="2.0"/>
+        <n v="3.0"/>
       </sharedItems>
     </cacheField>
     <cacheField name="groupName" numFmtId="0">
       <sharedItems>
         <s v="Первая"/>
         <s v="Вторая"/>
+        <s v="Третья"/>
       </sharedItems>
     </cacheField>
     <cacheField name="curator" numFmtId="0">
@@ -307,6 +317,7 @@
       <sharedItems>
         <s v="Создание собачек из человеков"/>
         <s v="Создание человеков из собачек"/>
+        <s v="Скрещивание собачек"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -315,7 +326,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Сводная таблица 1" cacheId="0" dataCaption="" rowGrandTotals="0">
-  <location ref="A1:D4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A1:E5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields>
     <pivotField name="student_id" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -325,6 +336,7 @@
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -336,6 +348,7 @@
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -347,6 +360,7 @@
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -358,6 +372,7 @@
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -369,6 +384,7 @@
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -376,6 +392,7 @@
       <items>
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -383,12 +400,14 @@
       <items>
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField name="educationYear" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
         <item x="0"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -396,6 +415,7 @@
       <items>
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -403,6 +423,7 @@
       <items>
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -417,6 +438,7 @@
       <items>
         <item x="0"/>
         <item x="1"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -740,6 +762,7 @@
     <row r="1"/>
     <row r="2"/>
     <row r="3"/>
+    <row r="4"/>
   </sheetData>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>